<commit_message>
Api Call is now fixed
</commit_message>
<xml_diff>
--- a/Timetable.xlsx
+++ b/Timetable.xlsx
@@ -1451,39 +1451,39 @@
       <c r="AU4" s="23" t="n"/>
       <c r="AV4" s="23" t="n"/>
       <c r="AW4" s="24" t="n"/>
-      <c r="AX4" s="25" t="n"/>
-      <c r="AY4" s="26" t="n"/>
-      <c r="AZ4" s="26" t="n"/>
-      <c r="BA4" s="26" t="n"/>
-      <c r="BB4" s="26" t="n"/>
-      <c r="BC4" s="26" t="n"/>
-      <c r="BD4" s="26" t="n"/>
-      <c r="BE4" s="26" t="n"/>
-      <c r="BF4" s="26" t="n"/>
-      <c r="BG4" s="26" t="n"/>
-      <c r="BH4" s="26" t="n"/>
-      <c r="BI4" s="27" t="n"/>
+      <c r="AX4" s="22" t="n"/>
+      <c r="AY4" s="23" t="n"/>
+      <c r="AZ4" s="23" t="n"/>
+      <c r="BA4" s="23" t="n"/>
+      <c r="BB4" s="23" t="n"/>
+      <c r="BC4" s="23" t="n"/>
+      <c r="BD4" s="23" t="n"/>
+      <c r="BE4" s="23" t="n"/>
+      <c r="BF4" s="23" t="n"/>
+      <c r="BG4" s="23" t="n"/>
+      <c r="BH4" s="23" t="n"/>
+      <c r="BI4" s="24" t="n"/>
       <c r="BJ4" s="22" t="n"/>
       <c r="BK4" s="23" t="n"/>
       <c r="BL4" s="23" t="n"/>
       <c r="BM4" s="23" t="n"/>
       <c r="BN4" s="23" t="n"/>
       <c r="BO4" s="23" t="n"/>
-      <c r="BP4" s="26" t="n"/>
-      <c r="BQ4" s="26" t="n"/>
-      <c r="BR4" s="26" t="n"/>
-      <c r="BS4" s="26" t="n"/>
-      <c r="BT4" s="26" t="n"/>
-      <c r="BU4" s="27" t="n"/>
-      <c r="BV4" s="25" t="n"/>
-      <c r="BW4" s="26" t="n"/>
-      <c r="BX4" s="26" t="n"/>
-      <c r="BY4" s="26" t="n"/>
-      <c r="BZ4" s="26" t="n"/>
-      <c r="CA4" s="26" t="n"/>
-      <c r="CB4" s="26" t="n"/>
-      <c r="CC4" s="26" t="n"/>
-      <c r="CD4" s="26" t="n"/>
+      <c r="BP4" s="23" t="n"/>
+      <c r="BQ4" s="23" t="n"/>
+      <c r="BR4" s="23" t="n"/>
+      <c r="BS4" s="23" t="n"/>
+      <c r="BT4" s="23" t="n"/>
+      <c r="BU4" s="24" t="n"/>
+      <c r="BV4" s="22" t="n"/>
+      <c r="BW4" s="23" t="n"/>
+      <c r="BX4" s="23" t="n"/>
+      <c r="BY4" s="23" t="n"/>
+      <c r="BZ4" s="23" t="n"/>
+      <c r="CA4" s="23" t="n"/>
+      <c r="CB4" s="23" t="n"/>
+      <c r="CC4" s="23" t="n"/>
+      <c r="CD4" s="23" t="n"/>
       <c r="CE4" s="23" t="n"/>
       <c r="CF4" s="23" t="n"/>
       <c r="CG4" s="24" t="n"/>
@@ -1674,18 +1674,18 @@
       <c r="BS5" s="23" t="n"/>
       <c r="BT5" s="23" t="n"/>
       <c r="BU5" s="24" t="n"/>
-      <c r="BV5" s="25" t="n"/>
-      <c r="BW5" s="26" t="n"/>
-      <c r="BX5" s="26" t="n"/>
-      <c r="BY5" s="26" t="n"/>
-      <c r="BZ5" s="26" t="n"/>
-      <c r="CA5" s="26" t="n"/>
-      <c r="CB5" s="26" t="n"/>
-      <c r="CC5" s="26" t="n"/>
-      <c r="CD5" s="26" t="n"/>
-      <c r="CE5" s="26" t="n"/>
-      <c r="CF5" s="26" t="n"/>
-      <c r="CG5" s="27" t="n"/>
+      <c r="BV5" s="22" t="n"/>
+      <c r="BW5" s="23" t="n"/>
+      <c r="BX5" s="23" t="n"/>
+      <c r="BY5" s="23" t="n"/>
+      <c r="BZ5" s="23" t="n"/>
+      <c r="CA5" s="23" t="n"/>
+      <c r="CB5" s="23" t="n"/>
+      <c r="CC5" s="23" t="n"/>
+      <c r="CD5" s="23" t="n"/>
+      <c r="CE5" s="23" t="n"/>
+      <c r="CF5" s="23" t="n"/>
+      <c r="CG5" s="24" t="n"/>
       <c r="CH5" s="22" t="n"/>
       <c r="CI5" s="23" t="n"/>
       <c r="CJ5" s="23" t="n"/>
@@ -1849,39 +1849,39 @@
       <c r="AU6" s="23" t="n"/>
       <c r="AV6" s="23" t="n"/>
       <c r="AW6" s="24" t="n"/>
-      <c r="AX6" s="25" t="n"/>
-      <c r="AY6" s="26" t="n"/>
-      <c r="AZ6" s="26" t="n"/>
-      <c r="BA6" s="26" t="n"/>
-      <c r="BB6" s="26" t="n"/>
-      <c r="BC6" s="26" t="n"/>
-      <c r="BD6" s="26" t="n"/>
-      <c r="BE6" s="26" t="n"/>
-      <c r="BF6" s="26" t="n"/>
-      <c r="BG6" s="26" t="n"/>
-      <c r="BH6" s="26" t="n"/>
-      <c r="BI6" s="27" t="n"/>
+      <c r="AX6" s="22" t="n"/>
+      <c r="AY6" s="23" t="n"/>
+      <c r="AZ6" s="23" t="n"/>
+      <c r="BA6" s="23" t="n"/>
+      <c r="BB6" s="23" t="n"/>
+      <c r="BC6" s="23" t="n"/>
+      <c r="BD6" s="23" t="n"/>
+      <c r="BE6" s="23" t="n"/>
+      <c r="BF6" s="23" t="n"/>
+      <c r="BG6" s="23" t="n"/>
+      <c r="BH6" s="23" t="n"/>
+      <c r="BI6" s="24" t="n"/>
       <c r="BJ6" s="22" t="n"/>
       <c r="BK6" s="23" t="n"/>
       <c r="BL6" s="23" t="n"/>
       <c r="BM6" s="23" t="n"/>
       <c r="BN6" s="23" t="n"/>
       <c r="BO6" s="23" t="n"/>
-      <c r="BP6" s="26" t="n"/>
-      <c r="BQ6" s="26" t="n"/>
-      <c r="BR6" s="26" t="n"/>
-      <c r="BS6" s="26" t="n"/>
-      <c r="BT6" s="26" t="n"/>
-      <c r="BU6" s="27" t="n"/>
-      <c r="BV6" s="25" t="n"/>
-      <c r="BW6" s="26" t="n"/>
-      <c r="BX6" s="26" t="n"/>
-      <c r="BY6" s="26" t="n"/>
-      <c r="BZ6" s="26" t="n"/>
-      <c r="CA6" s="26" t="n"/>
-      <c r="CB6" s="26" t="n"/>
-      <c r="CC6" s="26" t="n"/>
-      <c r="CD6" s="26" t="n"/>
+      <c r="BP6" s="23" t="n"/>
+      <c r="BQ6" s="23" t="n"/>
+      <c r="BR6" s="23" t="n"/>
+      <c r="BS6" s="23" t="n"/>
+      <c r="BT6" s="23" t="n"/>
+      <c r="BU6" s="24" t="n"/>
+      <c r="BV6" s="22" t="n"/>
+      <c r="BW6" s="23" t="n"/>
+      <c r="BX6" s="23" t="n"/>
+      <c r="BY6" s="23" t="n"/>
+      <c r="BZ6" s="23" t="n"/>
+      <c r="CA6" s="23" t="n"/>
+      <c r="CB6" s="23" t="n"/>
+      <c r="CC6" s="23" t="n"/>
+      <c r="CD6" s="23" t="n"/>
       <c r="CE6" s="23" t="n"/>
       <c r="CF6" s="23" t="n"/>
       <c r="CG6" s="24" t="n"/>
@@ -2048,18 +2048,18 @@
       <c r="AU7" s="23" t="n"/>
       <c r="AV7" s="23" t="n"/>
       <c r="AW7" s="24" t="n"/>
-      <c r="AX7" s="25" t="n"/>
-      <c r="AY7" s="26" t="n"/>
-      <c r="AZ7" s="26" t="n"/>
-      <c r="BA7" s="26" t="n"/>
-      <c r="BB7" s="26" t="n"/>
-      <c r="BC7" s="26" t="n"/>
-      <c r="BD7" s="26" t="n"/>
-      <c r="BE7" s="26" t="n"/>
-      <c r="BF7" s="26" t="n"/>
-      <c r="BG7" s="26" t="n"/>
-      <c r="BH7" s="26" t="n"/>
-      <c r="BI7" s="27" t="n"/>
+      <c r="AX7" s="22" t="n"/>
+      <c r="AY7" s="23" t="n"/>
+      <c r="AZ7" s="23" t="n"/>
+      <c r="BA7" s="23" t="n"/>
+      <c r="BB7" s="23" t="n"/>
+      <c r="BC7" s="23" t="n"/>
+      <c r="BD7" s="23" t="n"/>
+      <c r="BE7" s="23" t="n"/>
+      <c r="BF7" s="23" t="n"/>
+      <c r="BG7" s="23" t="n"/>
+      <c r="BH7" s="23" t="n"/>
+      <c r="BI7" s="24" t="n"/>
       <c r="BJ7" s="22" t="n"/>
       <c r="BK7" s="23" t="n"/>
       <c r="BL7" s="23" t="n"/>
@@ -2072,18 +2072,18 @@
       <c r="BS7" s="23" t="n"/>
       <c r="BT7" s="23" t="n"/>
       <c r="BU7" s="24" t="n"/>
-      <c r="BV7" s="25" t="n"/>
-      <c r="BW7" s="26" t="n"/>
-      <c r="BX7" s="26" t="n"/>
-      <c r="BY7" s="26" t="n"/>
-      <c r="BZ7" s="26" t="n"/>
-      <c r="CA7" s="26" t="n"/>
-      <c r="CB7" s="26" t="n"/>
-      <c r="CC7" s="26" t="n"/>
-      <c r="CD7" s="26" t="n"/>
-      <c r="CE7" s="26" t="n"/>
-      <c r="CF7" s="26" t="n"/>
-      <c r="CG7" s="27" t="n"/>
+      <c r="BV7" s="22" t="n"/>
+      <c r="BW7" s="23" t="n"/>
+      <c r="BX7" s="23" t="n"/>
+      <c r="BY7" s="23" t="n"/>
+      <c r="BZ7" s="23" t="n"/>
+      <c r="CA7" s="23" t="n"/>
+      <c r="CB7" s="23" t="n"/>
+      <c r="CC7" s="23" t="n"/>
+      <c r="CD7" s="23" t="n"/>
+      <c r="CE7" s="23" t="n"/>
+      <c r="CF7" s="23" t="n"/>
+      <c r="CG7" s="24" t="n"/>
       <c r="CH7" s="22" t="n"/>
       <c r="CI7" s="23" t="n"/>
       <c r="CJ7" s="23" t="n"/>
@@ -2247,39 +2247,39 @@
       <c r="AU8" s="23" t="n"/>
       <c r="AV8" s="23" t="n"/>
       <c r="AW8" s="24" t="n"/>
-      <c r="AX8" s="25" t="n"/>
-      <c r="AY8" s="26" t="n"/>
-      <c r="AZ8" s="26" t="n"/>
-      <c r="BA8" s="26" t="n"/>
-      <c r="BB8" s="26" t="n"/>
-      <c r="BC8" s="26" t="n"/>
-      <c r="BD8" s="26" t="n"/>
-      <c r="BE8" s="26" t="n"/>
-      <c r="BF8" s="26" t="n"/>
-      <c r="BG8" s="26" t="n"/>
-      <c r="BH8" s="26" t="n"/>
-      <c r="BI8" s="27" t="n"/>
+      <c r="AX8" s="22" t="n"/>
+      <c r="AY8" s="23" t="n"/>
+      <c r="AZ8" s="23" t="n"/>
+      <c r="BA8" s="23" t="n"/>
+      <c r="BB8" s="23" t="n"/>
+      <c r="BC8" s="23" t="n"/>
+      <c r="BD8" s="23" t="n"/>
+      <c r="BE8" s="23" t="n"/>
+      <c r="BF8" s="23" t="n"/>
+      <c r="BG8" s="23" t="n"/>
+      <c r="BH8" s="23" t="n"/>
+      <c r="BI8" s="24" t="n"/>
       <c r="BJ8" s="22" t="n"/>
       <c r="BK8" s="23" t="n"/>
       <c r="BL8" s="23" t="n"/>
       <c r="BM8" s="23" t="n"/>
       <c r="BN8" s="23" t="n"/>
       <c r="BO8" s="23" t="n"/>
-      <c r="BP8" s="26" t="n"/>
-      <c r="BQ8" s="26" t="n"/>
-      <c r="BR8" s="26" t="n"/>
-      <c r="BS8" s="26" t="n"/>
-      <c r="BT8" s="26" t="n"/>
-      <c r="BU8" s="27" t="n"/>
-      <c r="BV8" s="25" t="n"/>
-      <c r="BW8" s="26" t="n"/>
-      <c r="BX8" s="26" t="n"/>
-      <c r="BY8" s="26" t="n"/>
-      <c r="BZ8" s="26" t="n"/>
-      <c r="CA8" s="26" t="n"/>
-      <c r="CB8" s="26" t="n"/>
-      <c r="CC8" s="26" t="n"/>
-      <c r="CD8" s="26" t="n"/>
+      <c r="BP8" s="23" t="n"/>
+      <c r="BQ8" s="23" t="n"/>
+      <c r="BR8" s="23" t="n"/>
+      <c r="BS8" s="23" t="n"/>
+      <c r="BT8" s="23" t="n"/>
+      <c r="BU8" s="24" t="n"/>
+      <c r="BV8" s="22" t="n"/>
+      <c r="BW8" s="23" t="n"/>
+      <c r="BX8" s="23" t="n"/>
+      <c r="BY8" s="23" t="n"/>
+      <c r="BZ8" s="23" t="n"/>
+      <c r="CA8" s="23" t="n"/>
+      <c r="CB8" s="23" t="n"/>
+      <c r="CC8" s="23" t="n"/>
+      <c r="CD8" s="23" t="n"/>
       <c r="CE8" s="23" t="n"/>
       <c r="CF8" s="23" t="n"/>
       <c r="CG8" s="24" t="n"/>

</xml_diff>

<commit_message>
Updated OK Button External ID now updates on schedule source
</commit_message>
<xml_diff>
--- a/Timetable.xlsx
+++ b/Timetable.xlsx
@@ -1252,18 +1252,18 @@
       <c r="AU3" s="23" t="n"/>
       <c r="AV3" s="23" t="n"/>
       <c r="AW3" s="24" t="n"/>
-      <c r="AX3" s="22" t="n"/>
-      <c r="AY3" s="23" t="n"/>
-      <c r="AZ3" s="23" t="n"/>
-      <c r="BA3" s="23" t="n"/>
-      <c r="BB3" s="23" t="n"/>
-      <c r="BC3" s="23" t="n"/>
-      <c r="BD3" s="23" t="n"/>
-      <c r="BE3" s="23" t="n"/>
-      <c r="BF3" s="23" t="n"/>
-      <c r="BG3" s="23" t="n"/>
-      <c r="BH3" s="23" t="n"/>
-      <c r="BI3" s="24" t="n"/>
+      <c r="AX3" s="25" t="n"/>
+      <c r="AY3" s="26" t="n"/>
+      <c r="AZ3" s="26" t="n"/>
+      <c r="BA3" s="26" t="n"/>
+      <c r="BB3" s="26" t="n"/>
+      <c r="BC3" s="26" t="n"/>
+      <c r="BD3" s="26" t="n"/>
+      <c r="BE3" s="26" t="n"/>
+      <c r="BF3" s="26" t="n"/>
+      <c r="BG3" s="26" t="n"/>
+      <c r="BH3" s="26" t="n"/>
+      <c r="BI3" s="27" t="n"/>
       <c r="BJ3" s="22" t="n"/>
       <c r="BK3" s="23" t="n"/>
       <c r="BL3" s="23" t="n"/>

</xml_diff>

<commit_message>
Workday API client file has a hard coded version of class schedule
</commit_message>
<xml_diff>
--- a/Timetable.xlsx
+++ b/Timetable.xlsx
@@ -396,9 +396,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1485,42 +1485,42 @@
       <c r="AG4" s="39" t="n"/>
       <c r="AH4" s="39" t="n"/>
       <c r="AI4" s="39" t="n"/>
-      <c r="AJ4" s="41" t="n"/>
-      <c r="AK4" s="42" t="n"/>
-      <c r="AL4" s="43" t="n"/>
-      <c r="AM4" s="41" t="n"/>
-      <c r="AN4" s="41" t="n"/>
-      <c r="AO4" s="41" t="n"/>
-      <c r="AP4" s="41" t="n"/>
-      <c r="AQ4" s="41" t="n"/>
-      <c r="AR4" s="41" t="n"/>
-      <c r="AS4" s="41" t="n"/>
+      <c r="AJ4" s="39" t="n"/>
+      <c r="AK4" s="40" t="n"/>
+      <c r="AL4" s="38" t="n"/>
+      <c r="AM4" s="39" t="n"/>
+      <c r="AN4" s="39" t="n"/>
+      <c r="AO4" s="39" t="n"/>
+      <c r="AP4" s="39" t="n"/>
+      <c r="AQ4" s="39" t="n"/>
+      <c r="AR4" s="39" t="n"/>
+      <c r="AS4" s="39" t="n"/>
       <c r="AT4" s="39" t="n"/>
       <c r="AU4" s="39" t="n"/>
       <c r="AV4" s="39" t="n"/>
-      <c r="AW4" s="42" t="n"/>
-      <c r="AX4" s="43" t="n"/>
-      <c r="AY4" s="41" t="n"/>
-      <c r="AZ4" s="41" t="n"/>
-      <c r="BA4" s="41" t="n"/>
-      <c r="BB4" s="41" t="n"/>
-      <c r="BC4" s="41" t="n"/>
-      <c r="BD4" s="41" t="n"/>
-      <c r="BE4" s="41" t="n"/>
-      <c r="BF4" s="41" t="n"/>
+      <c r="AW4" s="40" t="n"/>
+      <c r="AX4" s="38" t="n"/>
+      <c r="AY4" s="39" t="n"/>
+      <c r="AZ4" s="39" t="n"/>
+      <c r="BA4" s="39" t="n"/>
+      <c r="BB4" s="39" t="n"/>
+      <c r="BC4" s="39" t="n"/>
+      <c r="BD4" s="39" t="n"/>
+      <c r="BE4" s="39" t="n"/>
+      <c r="BF4" s="39" t="n"/>
       <c r="BG4" s="39" t="n"/>
       <c r="BH4" s="39" t="n"/>
       <c r="BI4" s="40" t="n"/>
-      <c r="BJ4" s="43" t="n"/>
-      <c r="BK4" s="41" t="n"/>
-      <c r="BL4" s="41" t="n"/>
-      <c r="BM4" s="41" t="n"/>
-      <c r="BN4" s="41" t="n"/>
-      <c r="BO4" s="41" t="n"/>
-      <c r="BP4" s="41" t="n"/>
-      <c r="BQ4" s="41" t="n"/>
-      <c r="BR4" s="41" t="n"/>
-      <c r="BS4" s="41" t="n"/>
+      <c r="BJ4" s="38" t="n"/>
+      <c r="BK4" s="39" t="n"/>
+      <c r="BL4" s="39" t="n"/>
+      <c r="BM4" s="39" t="n"/>
+      <c r="BN4" s="39" t="n"/>
+      <c r="BO4" s="39" t="n"/>
+      <c r="BP4" s="39" t="n"/>
+      <c r="BQ4" s="39" t="n"/>
+      <c r="BR4" s="39" t="n"/>
+      <c r="BS4" s="39" t="n"/>
       <c r="BT4" s="39" t="n"/>
       <c r="BU4" s="40" t="n"/>
       <c r="BV4" s="38" t="n"/>
@@ -1563,16 +1563,16 @@
       <c r="DG4" s="39" t="n"/>
       <c r="DH4" s="39" t="n"/>
       <c r="DI4" s="39" t="n"/>
-      <c r="DJ4" s="41" t="n"/>
-      <c r="DK4" s="41" t="n"/>
-      <c r="DL4" s="41" t="n"/>
-      <c r="DM4" s="41" t="n"/>
-      <c r="DN4" s="41" t="n"/>
-      <c r="DO4" s="41" t="n"/>
-      <c r="DP4" s="41" t="n"/>
-      <c r="DQ4" s="42" t="n"/>
-      <c r="DR4" s="43" t="n"/>
-      <c r="DS4" s="41" t="n"/>
+      <c r="DJ4" s="39" t="n"/>
+      <c r="DK4" s="39" t="n"/>
+      <c r="DL4" s="39" t="n"/>
+      <c r="DM4" s="39" t="n"/>
+      <c r="DN4" s="39" t="n"/>
+      <c r="DO4" s="39" t="n"/>
+      <c r="DP4" s="39" t="n"/>
+      <c r="DQ4" s="40" t="n"/>
+      <c r="DR4" s="38" t="n"/>
+      <c r="DS4" s="39" t="n"/>
       <c r="DT4" s="39" t="n"/>
       <c r="DU4" s="39" t="n"/>
       <c r="DV4" s="39" t="n"/>
@@ -1758,30 +1758,30 @@
       <c r="DC5" s="39" t="n"/>
       <c r="DD5" s="39" t="n"/>
       <c r="DE5" s="40" t="n"/>
-      <c r="DF5" s="38" t="n"/>
-      <c r="DG5" s="39" t="n"/>
-      <c r="DH5" s="41" t="n"/>
-      <c r="DI5" s="41" t="n"/>
-      <c r="DJ5" s="41" t="n"/>
-      <c r="DK5" s="41" t="n"/>
-      <c r="DL5" s="41" t="n"/>
-      <c r="DM5" s="41" t="n"/>
-      <c r="DN5" s="41" t="n"/>
-      <c r="DO5" s="41" t="n"/>
-      <c r="DP5" s="41" t="n"/>
-      <c r="DQ5" s="42" t="n"/>
-      <c r="DR5" s="38" t="n"/>
-      <c r="DS5" s="39" t="n"/>
-      <c r="DT5" s="39" t="n"/>
-      <c r="DU5" s="39" t="n"/>
-      <c r="DV5" s="39" t="n"/>
-      <c r="DW5" s="39" t="n"/>
-      <c r="DX5" s="39" t="n"/>
-      <c r="DY5" s="39" t="n"/>
-      <c r="DZ5" s="39" t="n"/>
-      <c r="EA5" s="39" t="n"/>
-      <c r="EB5" s="39" t="n"/>
-      <c r="EC5" s="40" t="n"/>
+      <c r="DF5" s="41" t="n"/>
+      <c r="DG5" s="42" t="n"/>
+      <c r="DH5" s="42" t="n"/>
+      <c r="DI5" s="42" t="n"/>
+      <c r="DJ5" s="42" t="n"/>
+      <c r="DK5" s="42" t="n"/>
+      <c r="DL5" s="42" t="n"/>
+      <c r="DM5" s="42" t="n"/>
+      <c r="DN5" s="42" t="n"/>
+      <c r="DO5" s="42" t="n"/>
+      <c r="DP5" s="42" t="n"/>
+      <c r="DQ5" s="43" t="n"/>
+      <c r="DR5" s="41" t="n"/>
+      <c r="DS5" s="42" t="n"/>
+      <c r="DT5" s="42" t="n"/>
+      <c r="DU5" s="42" t="n"/>
+      <c r="DV5" s="42" t="n"/>
+      <c r="DW5" s="42" t="n"/>
+      <c r="DX5" s="42" t="n"/>
+      <c r="DY5" s="42" t="n"/>
+      <c r="DZ5" s="42" t="n"/>
+      <c r="EA5" s="42" t="n"/>
+      <c r="EB5" s="42" t="n"/>
+      <c r="EC5" s="43" t="n"/>
       <c r="ED5" s="38" t="n"/>
       <c r="EE5" s="39" t="n"/>
       <c r="EF5" s="39" t="n"/>
@@ -1883,42 +1883,42 @@
       <c r="AG6" s="39" t="n"/>
       <c r="AH6" s="39" t="n"/>
       <c r="AI6" s="39" t="n"/>
-      <c r="AJ6" s="41" t="n"/>
-      <c r="AK6" s="42" t="n"/>
-      <c r="AL6" s="43" t="n"/>
-      <c r="AM6" s="41" t="n"/>
-      <c r="AN6" s="41" t="n"/>
-      <c r="AO6" s="41" t="n"/>
-      <c r="AP6" s="41" t="n"/>
-      <c r="AQ6" s="41" t="n"/>
-      <c r="AR6" s="41" t="n"/>
-      <c r="AS6" s="41" t="n"/>
+      <c r="AJ6" s="39" t="n"/>
+      <c r="AK6" s="40" t="n"/>
+      <c r="AL6" s="38" t="n"/>
+      <c r="AM6" s="39" t="n"/>
+      <c r="AN6" s="39" t="n"/>
+      <c r="AO6" s="39" t="n"/>
+      <c r="AP6" s="39" t="n"/>
+      <c r="AQ6" s="39" t="n"/>
+      <c r="AR6" s="39" t="n"/>
+      <c r="AS6" s="39" t="n"/>
       <c r="AT6" s="39" t="n"/>
       <c r="AU6" s="39" t="n"/>
       <c r="AV6" s="39" t="n"/>
-      <c r="AW6" s="42" t="n"/>
-      <c r="AX6" s="43" t="n"/>
-      <c r="AY6" s="41" t="n"/>
-      <c r="AZ6" s="41" t="n"/>
-      <c r="BA6" s="41" t="n"/>
-      <c r="BB6" s="41" t="n"/>
-      <c r="BC6" s="41" t="n"/>
-      <c r="BD6" s="41" t="n"/>
-      <c r="BE6" s="41" t="n"/>
-      <c r="BF6" s="41" t="n"/>
+      <c r="AW6" s="40" t="n"/>
+      <c r="AX6" s="38" t="n"/>
+      <c r="AY6" s="39" t="n"/>
+      <c r="AZ6" s="39" t="n"/>
+      <c r="BA6" s="39" t="n"/>
+      <c r="BB6" s="39" t="n"/>
+      <c r="BC6" s="39" t="n"/>
+      <c r="BD6" s="39" t="n"/>
+      <c r="BE6" s="39" t="n"/>
+      <c r="BF6" s="39" t="n"/>
       <c r="BG6" s="39" t="n"/>
       <c r="BH6" s="39" t="n"/>
       <c r="BI6" s="40" t="n"/>
-      <c r="BJ6" s="43" t="n"/>
-      <c r="BK6" s="41" t="n"/>
-      <c r="BL6" s="41" t="n"/>
-      <c r="BM6" s="41" t="n"/>
-      <c r="BN6" s="41" t="n"/>
-      <c r="BO6" s="41" t="n"/>
-      <c r="BP6" s="41" t="n"/>
-      <c r="BQ6" s="41" t="n"/>
-      <c r="BR6" s="41" t="n"/>
-      <c r="BS6" s="41" t="n"/>
+      <c r="BJ6" s="38" t="n"/>
+      <c r="BK6" s="39" t="n"/>
+      <c r="BL6" s="39" t="n"/>
+      <c r="BM6" s="39" t="n"/>
+      <c r="BN6" s="39" t="n"/>
+      <c r="BO6" s="39" t="n"/>
+      <c r="BP6" s="39" t="n"/>
+      <c r="BQ6" s="39" t="n"/>
+      <c r="BR6" s="39" t="n"/>
+      <c r="BS6" s="39" t="n"/>
       <c r="BT6" s="39" t="n"/>
       <c r="BU6" s="40" t="n"/>
       <c r="BV6" s="38" t="n"/>
@@ -1961,16 +1961,16 @@
       <c r="DG6" s="39" t="n"/>
       <c r="DH6" s="39" t="n"/>
       <c r="DI6" s="39" t="n"/>
-      <c r="DJ6" s="41" t="n"/>
-      <c r="DK6" s="41" t="n"/>
-      <c r="DL6" s="41" t="n"/>
-      <c r="DM6" s="41" t="n"/>
-      <c r="DN6" s="41" t="n"/>
-      <c r="DO6" s="41" t="n"/>
-      <c r="DP6" s="41" t="n"/>
-      <c r="DQ6" s="42" t="n"/>
-      <c r="DR6" s="43" t="n"/>
-      <c r="DS6" s="41" t="n"/>
+      <c r="DJ6" s="39" t="n"/>
+      <c r="DK6" s="39" t="n"/>
+      <c r="DL6" s="39" t="n"/>
+      <c r="DM6" s="39" t="n"/>
+      <c r="DN6" s="39" t="n"/>
+      <c r="DO6" s="39" t="n"/>
+      <c r="DP6" s="39" t="n"/>
+      <c r="DQ6" s="40" t="n"/>
+      <c r="DR6" s="38" t="n"/>
+      <c r="DS6" s="39" t="n"/>
       <c r="DT6" s="39" t="n"/>
       <c r="DU6" s="39" t="n"/>
       <c r="DV6" s="39" t="n"/>
@@ -2146,52 +2146,52 @@
       <c r="CS7" s="40" t="n"/>
       <c r="CT7" s="38" t="n"/>
       <c r="CU7" s="39" t="n"/>
-      <c r="CV7" s="41" t="n"/>
-      <c r="CW7" s="41" t="n"/>
-      <c r="CX7" s="41" t="n"/>
-      <c r="CY7" s="41" t="n"/>
-      <c r="CZ7" s="41" t="n"/>
-      <c r="DA7" s="41" t="n"/>
-      <c r="DB7" s="41" t="n"/>
-      <c r="DC7" s="41" t="n"/>
-      <c r="DD7" s="41" t="n"/>
-      <c r="DE7" s="42" t="n"/>
-      <c r="DF7" s="38" t="n"/>
-      <c r="DG7" s="39" t="n"/>
-      <c r="DH7" s="41" t="n"/>
-      <c r="DI7" s="41" t="n"/>
-      <c r="DJ7" s="41" t="n"/>
-      <c r="DK7" s="41" t="n"/>
-      <c r="DL7" s="41" t="n"/>
-      <c r="DM7" s="41" t="n"/>
-      <c r="DN7" s="41" t="n"/>
-      <c r="DO7" s="41" t="n"/>
-      <c r="DP7" s="41" t="n"/>
-      <c r="DQ7" s="42" t="n"/>
-      <c r="DR7" s="38" t="n"/>
-      <c r="DS7" s="39" t="n"/>
-      <c r="DT7" s="41" t="n"/>
-      <c r="DU7" s="41" t="n"/>
-      <c r="DV7" s="41" t="n"/>
-      <c r="DW7" s="41" t="n"/>
-      <c r="DX7" s="41" t="n"/>
-      <c r="DY7" s="41" t="n"/>
-      <c r="DZ7" s="41" t="n"/>
-      <c r="EA7" s="41" t="n"/>
-      <c r="EB7" s="41" t="n"/>
-      <c r="EC7" s="42" t="n"/>
-      <c r="ED7" s="43" t="n"/>
-      <c r="EE7" s="41" t="n"/>
-      <c r="EF7" s="41" t="n"/>
-      <c r="EG7" s="41" t="n"/>
-      <c r="EH7" s="41" t="n"/>
-      <c r="EI7" s="41" t="n"/>
-      <c r="EJ7" s="41" t="n"/>
-      <c r="EK7" s="41" t="n"/>
-      <c r="EL7" s="41" t="n"/>
-      <c r="EM7" s="41" t="n"/>
-      <c r="EN7" s="41" t="n"/>
-      <c r="EO7" s="42" t="n"/>
+      <c r="CV7" s="39" t="n"/>
+      <c r="CW7" s="39" t="n"/>
+      <c r="CX7" s="39" t="n"/>
+      <c r="CY7" s="39" t="n"/>
+      <c r="CZ7" s="39" t="n"/>
+      <c r="DA7" s="39" t="n"/>
+      <c r="DB7" s="39" t="n"/>
+      <c r="DC7" s="39" t="n"/>
+      <c r="DD7" s="39" t="n"/>
+      <c r="DE7" s="40" t="n"/>
+      <c r="DF7" s="41" t="n"/>
+      <c r="DG7" s="42" t="n"/>
+      <c r="DH7" s="42" t="n"/>
+      <c r="DI7" s="42" t="n"/>
+      <c r="DJ7" s="42" t="n"/>
+      <c r="DK7" s="42" t="n"/>
+      <c r="DL7" s="42" t="n"/>
+      <c r="DM7" s="42" t="n"/>
+      <c r="DN7" s="42" t="n"/>
+      <c r="DO7" s="42" t="n"/>
+      <c r="DP7" s="42" t="n"/>
+      <c r="DQ7" s="43" t="n"/>
+      <c r="DR7" s="41" t="n"/>
+      <c r="DS7" s="42" t="n"/>
+      <c r="DT7" s="42" t="n"/>
+      <c r="DU7" s="42" t="n"/>
+      <c r="DV7" s="42" t="n"/>
+      <c r="DW7" s="42" t="n"/>
+      <c r="DX7" s="42" t="n"/>
+      <c r="DY7" s="42" t="n"/>
+      <c r="DZ7" s="42" t="n"/>
+      <c r="EA7" s="42" t="n"/>
+      <c r="EB7" s="42" t="n"/>
+      <c r="EC7" s="43" t="n"/>
+      <c r="ED7" s="38" t="n"/>
+      <c r="EE7" s="39" t="n"/>
+      <c r="EF7" s="39" t="n"/>
+      <c r="EG7" s="39" t="n"/>
+      <c r="EH7" s="39" t="n"/>
+      <c r="EI7" s="39" t="n"/>
+      <c r="EJ7" s="39" t="n"/>
+      <c r="EK7" s="39" t="n"/>
+      <c r="EL7" s="39" t="n"/>
+      <c r="EM7" s="39" t="n"/>
+      <c r="EN7" s="39" t="n"/>
+      <c r="EO7" s="40" t="n"/>
       <c r="EP7" s="38" t="n"/>
       <c r="EQ7" s="39" t="n"/>
       <c r="ER7" s="39" t="n"/>
@@ -2281,42 +2281,42 @@
       <c r="AG8" s="39" t="n"/>
       <c r="AH8" s="39" t="n"/>
       <c r="AI8" s="39" t="n"/>
-      <c r="AJ8" s="41" t="n"/>
-      <c r="AK8" s="42" t="n"/>
-      <c r="AL8" s="43" t="n"/>
-      <c r="AM8" s="41" t="n"/>
-      <c r="AN8" s="41" t="n"/>
-      <c r="AO8" s="41" t="n"/>
-      <c r="AP8" s="41" t="n"/>
-      <c r="AQ8" s="41" t="n"/>
-      <c r="AR8" s="41" t="n"/>
-      <c r="AS8" s="41" t="n"/>
+      <c r="AJ8" s="39" t="n"/>
+      <c r="AK8" s="40" t="n"/>
+      <c r="AL8" s="38" t="n"/>
+      <c r="AM8" s="39" t="n"/>
+      <c r="AN8" s="39" t="n"/>
+      <c r="AO8" s="39" t="n"/>
+      <c r="AP8" s="39" t="n"/>
+      <c r="AQ8" s="39" t="n"/>
+      <c r="AR8" s="39" t="n"/>
+      <c r="AS8" s="39" t="n"/>
       <c r="AT8" s="39" t="n"/>
       <c r="AU8" s="39" t="n"/>
       <c r="AV8" s="39" t="n"/>
-      <c r="AW8" s="42" t="n"/>
-      <c r="AX8" s="43" t="n"/>
-      <c r="AY8" s="41" t="n"/>
-      <c r="AZ8" s="41" t="n"/>
-      <c r="BA8" s="41" t="n"/>
-      <c r="BB8" s="41" t="n"/>
-      <c r="BC8" s="41" t="n"/>
-      <c r="BD8" s="41" t="n"/>
-      <c r="BE8" s="41" t="n"/>
-      <c r="BF8" s="41" t="n"/>
+      <c r="AW8" s="40" t="n"/>
+      <c r="AX8" s="38" t="n"/>
+      <c r="AY8" s="39" t="n"/>
+      <c r="AZ8" s="39" t="n"/>
+      <c r="BA8" s="39" t="n"/>
+      <c r="BB8" s="39" t="n"/>
+      <c r="BC8" s="39" t="n"/>
+      <c r="BD8" s="39" t="n"/>
+      <c r="BE8" s="39" t="n"/>
+      <c r="BF8" s="39" t="n"/>
       <c r="BG8" s="39" t="n"/>
       <c r="BH8" s="39" t="n"/>
       <c r="BI8" s="40" t="n"/>
-      <c r="BJ8" s="43" t="n"/>
-      <c r="BK8" s="41" t="n"/>
-      <c r="BL8" s="41" t="n"/>
-      <c r="BM8" s="41" t="n"/>
-      <c r="BN8" s="41" t="n"/>
-      <c r="BO8" s="41" t="n"/>
-      <c r="BP8" s="41" t="n"/>
-      <c r="BQ8" s="41" t="n"/>
-      <c r="BR8" s="41" t="n"/>
-      <c r="BS8" s="41" t="n"/>
+      <c r="BJ8" s="38" t="n"/>
+      <c r="BK8" s="39" t="n"/>
+      <c r="BL8" s="39" t="n"/>
+      <c r="BM8" s="39" t="n"/>
+      <c r="BN8" s="39" t="n"/>
+      <c r="BO8" s="39" t="n"/>
+      <c r="BP8" s="39" t="n"/>
+      <c r="BQ8" s="39" t="n"/>
+      <c r="BR8" s="39" t="n"/>
+      <c r="BS8" s="39" t="n"/>
       <c r="BT8" s="39" t="n"/>
       <c r="BU8" s="40" t="n"/>
       <c r="BV8" s="38" t="n"/>
@@ -2359,16 +2359,16 @@
       <c r="DG8" s="39" t="n"/>
       <c r="DH8" s="39" t="n"/>
       <c r="DI8" s="39" t="n"/>
-      <c r="DJ8" s="41" t="n"/>
-      <c r="DK8" s="41" t="n"/>
-      <c r="DL8" s="41" t="n"/>
-      <c r="DM8" s="41" t="n"/>
-      <c r="DN8" s="41" t="n"/>
-      <c r="DO8" s="41" t="n"/>
-      <c r="DP8" s="41" t="n"/>
-      <c r="DQ8" s="42" t="n"/>
-      <c r="DR8" s="43" t="n"/>
-      <c r="DS8" s="41" t="n"/>
+      <c r="DJ8" s="39" t="n"/>
+      <c r="DK8" s="39" t="n"/>
+      <c r="DL8" s="39" t="n"/>
+      <c r="DM8" s="39" t="n"/>
+      <c r="DN8" s="39" t="n"/>
+      <c r="DO8" s="39" t="n"/>
+      <c r="DP8" s="39" t="n"/>
+      <c r="DQ8" s="40" t="n"/>
+      <c r="DR8" s="38" t="n"/>
+      <c r="DS8" s="39" t="n"/>
       <c r="DT8" s="39" t="n"/>
       <c r="DU8" s="39" t="n"/>
       <c r="DV8" s="39" t="n"/>

</xml_diff>